<commit_message>
updated general MC for mid-Atlantic
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/general_monte_carlo/user_inputs_general_monte_carlo.xlsx
+++ b/projects/mid_atlantic/general_monte_carlo/user_inputs_general_monte_carlo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592DAF5C-2A97-478A-8584-10B0AF7471E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75B10B4-D172-4E96-838F-998BB2E76FF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed_diameter" sheetId="10" r:id="rId1"/>
@@ -532,779 +532,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33148202-7FD3-419C-810B-5ECE05747F7D}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1402.35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>1005.84</v>
-      </c>
-      <c r="F2">
-        <v>5554.43</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3">
-        <v>62.44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1225.0060000000001</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.22919999999999999</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>0.18559999999999999</v>
-      </c>
-      <c r="F4">
-        <v>0.37140000000000001</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>0.01</v>
-      </c>
-      <c r="F5">
-        <v>5000</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="8">
-        <v>200</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="8">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8">
-        <v>650</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="8">
-        <v>200</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="8">
-        <v>5</v>
-      </c>
-      <c r="F7" s="8">
-        <v>550</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="5">
-        <v>16.850000000000001</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.101325</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="5">
-        <v>16.850000000000001</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0.101325</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="5">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="5">
-        <v>14.73</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2.4201667441120001E-2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="6">
-        <v>7.4124359999999996</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="5">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="12">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="8">
-        <v>0</v>
-      </c>
-      <c r="G19" s="8">
-        <v>0</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="8">
-        <v>0</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="11">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="8">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8">
-        <v>0</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="8">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8">
-        <v>0</v>
-      </c>
-      <c r="G22" s="8">
-        <v>0</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="8">
-        <v>0</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0</v>
-      </c>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="8">
-        <v>1</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="8">
-        <v>0</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0</v>
-      </c>
-      <c r="G24" s="8">
-        <v>0</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="8">
-        <v>1</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="8">
-        <v>0</v>
-      </c>
-      <c r="F25" s="8">
-        <v>0</v>
-      </c>
-      <c r="G25" s="8">
-        <v>0</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="8">
-        <v>1</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="8">
-        <v>0</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0</v>
-      </c>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="8">
-        <v>1</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="8">
-        <v>0</v>
-      </c>
-      <c r="F27" s="8">
-        <v>0</v>
-      </c>
-      <c r="G27" s="8">
-        <v>0</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="8">
-        <v>1</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="8">
-        <v>0</v>
-      </c>
-      <c r="F28" s="8">
-        <v>0</v>
-      </c>
-      <c r="G28" s="8">
-        <v>0</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="8">
-        <v>1</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" s="8">
-        <v>0</v>
-      </c>
-      <c r="F29" s="8">
-        <v>0</v>
-      </c>
-      <c r="G29" s="8">
-        <v>0</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
@@ -1659,6 +886,779 @@
       <c r="B14" t="s">
         <v>46</v>
       </c>
+      <c r="C14" s="5">
+        <v>14.73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2.4201667441120001E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="6">
+        <v>7.4124359999999996</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="11">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0</v>
+      </c>
+      <c r="G28" s="8">
+        <v>0</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0</v>
+      </c>
+      <c r="G29" s="8">
+        <v>0</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1402.35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2">
+        <v>2000</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>62.44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.22919999999999999</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>0.2</v>
+      </c>
+      <c r="F4">
+        <v>0.4</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="8">
+        <v>200</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>650</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8">
+        <v>200</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8">
+        <v>550</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="5">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.101325</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="5">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.101325</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="5">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
       <c r="C14" s="7">
         <v>14.73</v>
       </c>

</xml_diff>

<commit_message>
Updated Mach limit based on model equations
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/general_monte_carlo/user_inputs_general_monte_carlo.xlsx
+++ b/projects/mid_atlantic/general_monte_carlo/user_inputs_general_monte_carlo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75B10B4-D172-4E96-838F-998BB2E76FF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF2BB6F-D188-45BE-8BF3-F6E1E0295F36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed_diameter" sheetId="10" r:id="rId1"/>
@@ -1306,7 +1306,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,10 +1460,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="8">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="F6" s="8">
-        <v>650</v>
+        <v>500</v>
       </c>
       <c r="G6" s="8">
         <v>0</v>
@@ -1486,10 +1486,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F7" s="8">
-        <v>550</v>
+        <v>100</v>
       </c>
       <c r="G7" s="8">
         <v>0</v>

</xml_diff>